<commit_message>
add the adversarial training model and results in demo_mnist/new_adversarial_examples/
</commit_message>
<xml_diff>
--- a/demo_mnist/new_adversarial_examples/result.xlsx
+++ b/demo_mnist/new_adversarial_examples/result.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9D38E1-E1FC-4F59-B368-346FB0BDAC6F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE57C13B-C350-4D27-BE76-20EF2ACA3FA6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>LAT_model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,6 +87,14 @@
   </si>
   <si>
     <t>pro_num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adv_training_model(eps=0.2,alpha = 0.5)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>adv_training_model(eps=0.1,alpha = 0.5)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -420,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -431,17 +439,24 @@
     <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -451,8 +466,14 @@
       <c r="C2">
         <v>0.97</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>0.97</v>
+      </c>
+      <c r="E2">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -462,8 +483,14 @@
       <c r="C3">
         <v>0.72</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0.97</v>
+      </c>
+      <c r="E3">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -473,8 +500,14 @@
       <c r="C4">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0.97</v>
+      </c>
+      <c r="E4">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -484,8 +517,14 @@
       <c r="C5">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0.95</v>
+      </c>
+      <c r="E5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -493,7 +532,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -501,7 +540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -509,7 +548,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -517,7 +556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -525,7 +564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -533,7 +572,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -541,7 +580,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -549,7 +588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -557,7 +596,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
modified code in adversarial_training.py
</commit_message>
<xml_diff>
--- a/demo_mnist/new_adversarial_examples/result.xlsx
+++ b/demo_mnist/new_adversarial_examples/result.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE57C13B-C350-4D27-BE76-20EF2ACA3FA6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D10F58-C8F7-42E6-98B2-7AE4ADB58AE5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -521,7 +521,7 @@
         <v>0.95</v>
       </c>
       <c r="E5">
-        <v>0.81</v>
+        <v>0.78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>